<commit_message>
the grid to gsc_algorithm
</commit_message>
<xml_diff>
--- a/participants_preferences.xlsx
+++ b/participants_preferences.xlsx
@@ -5,23 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pascal/PycharmProjects/labor_rotation_algorithms/excelsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pascal/PycharmProjects/internal-labor-rotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28ADE6D2-FF2B-DD4D-A0A9-5A15FF752FA3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1EBEDD-AAD9-CF4A-9028-2E6950822A10}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="18440" windowHeight="19760" activeTab="1" xr2:uid="{DCF1C8F3-97A6-AD46-8D67-C6CB5B41C1F9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="The grid" sheetId="4" r:id="rId4"/>
-    <sheet name="test" sheetId="5" r:id="rId5"/>
+    <sheet name="list_of_participants" sheetId="6" r:id="rId1"/>
+    <sheet name="Workers" sheetId="1" r:id="rId2"/>
+    <sheet name="Managers" sheetId="2" r:id="rId3"/>
+    <sheet name="Grid" sheetId="3" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName name="result" localSheetId="4">test!$A$1:$C$6</definedName>
-  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,22 +27,8 @@
 </workbook>
 </file>
 
-<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="result" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr sourceFile="/Users/pascal/PycharmProjects/test_1/excelsheets/result.txt" decimal="," thousands="." comma="1">
-      <textFields count="3">
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-</connections>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="29">
   <si>
     <t>Rank</t>
   </si>
@@ -75,18 +57,6 @@
     <t>w5</t>
   </si>
   <si>
-    <t>j1</t>
-  </si>
-  <si>
-    <t>j2</t>
-  </si>
-  <si>
-    <t>Was not proposed to.</t>
-  </si>
-  <si>
-    <t>No match</t>
-  </si>
-  <si>
     <t>j12</t>
   </si>
   <si>
@@ -112,6 +82,39 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>List of workers</t>
+  </si>
+  <si>
+    <t>List of Managers</t>
+  </si>
+  <si>
+    <t>w6</t>
+  </si>
+  <si>
+    <t>w7</t>
+  </si>
+  <si>
+    <t>w8</t>
+  </si>
+  <si>
+    <t>w9</t>
+  </si>
+  <si>
+    <t>w10</t>
+  </si>
+  <si>
+    <t>w11</t>
+  </si>
+  <si>
+    <t>w12</t>
+  </si>
+  <si>
+    <t>w13</t>
+  </si>
+  <si>
+    <t>w14</t>
   </si>
 </sst>
 </file>
@@ -297,10 +300,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result" connectionId="1" xr16:uid="{00000000-0016-0000-0400-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -599,11 +598,107 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDD478F1-64C1-104C-8378-10097C1996F9}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView zoomScale="50" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="2" width="31.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{596F157E-26D9-BE4C-8920-4F34520429A5}">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.33203125" defaultRowHeight="16"/>
@@ -632,19 +727,19 @@
     </row>
     <row r="2" spans="1:15" s="14" customFormat="1" ht="23" customHeight="1">
       <c r="A2" s="13" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>17</v>
-      </c>
       <c r="E2" s="13" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
@@ -659,19 +754,19 @@
     </row>
     <row r="3" spans="1:15" s="14" customFormat="1" ht="23" customHeight="1">
       <c r="A3" s="13" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
@@ -689,16 +784,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
@@ -716,16 +811,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
@@ -743,16 +838,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -771,7 +866,7 @@
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E7" s="10"/>
     </row>
@@ -790,12 +885,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6140E9A8-F7FE-D04B-9D22-29E6F982C507}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView zoomScale="177" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.6640625" defaultRowHeight="16"/>
@@ -808,24 +903,24 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C1" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="16" t="s">
-        <v>17</v>
-      </c>
       <c r="E1" s="16" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="17" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="16" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>4</v>
@@ -937,7 +1032,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D7C2C3-ECF9-554C-BEA6-437A84A51C27}">
   <dimension ref="A1:C111"/>
   <sheetViews>
@@ -1799,806 +1894,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58E88EA1-6A21-A442-92A5-251FDC849175}">
-  <dimension ref="A1:C64"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5">
-        <v>2</v>
-      </c>
-      <c r="C4" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5">
-        <v>2</v>
-      </c>
-      <c r="C6" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="5">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5">
-        <v>3</v>
-      </c>
-      <c r="C7" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="5">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6">
-        <v>1</v>
-      </c>
-      <c r="C8" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="5">
-        <v>8</v>
-      </c>
-      <c r="B9" s="6">
-        <v>2</v>
-      </c>
-      <c r="C9" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="5">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6">
-        <v>3</v>
-      </c>
-      <c r="C10" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="5">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6">
-        <v>4</v>
-      </c>
-      <c r="C11" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="5">
-        <v>11</v>
-      </c>
-      <c r="B12" s="6">
-        <v>1</v>
-      </c>
-      <c r="C12" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="5">
-        <v>12</v>
-      </c>
-      <c r="B13" s="6">
-        <v>2</v>
-      </c>
-      <c r="C13" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="5">
-        <v>13</v>
-      </c>
-      <c r="B14" s="6">
-        <v>3</v>
-      </c>
-      <c r="C14" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="5">
-        <v>14</v>
-      </c>
-      <c r="B15" s="6">
-        <v>4</v>
-      </c>
-      <c r="C15" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="5">
-        <v>15</v>
-      </c>
-      <c r="B16" s="6">
-        <v>5</v>
-      </c>
-      <c r="C16" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="5">
-        <v>16</v>
-      </c>
-      <c r="B17" s="6">
-        <v>1</v>
-      </c>
-      <c r="C17" s="6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="5">
-        <v>17</v>
-      </c>
-      <c r="B18" s="6">
-        <v>2</v>
-      </c>
-      <c r="C18" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="5">
-        <v>18</v>
-      </c>
-      <c r="B19" s="6">
-        <v>3</v>
-      </c>
-      <c r="C19" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="5">
-        <v>19</v>
-      </c>
-      <c r="B20" s="6">
-        <v>4</v>
-      </c>
-      <c r="C20" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="5">
-        <v>20</v>
-      </c>
-      <c r="B21" s="6">
-        <v>5</v>
-      </c>
-      <c r="C21" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="5">
-        <v>21</v>
-      </c>
-      <c r="B22" s="6">
-        <v>6</v>
-      </c>
-      <c r="C22" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="5">
-        <v>22</v>
-      </c>
-      <c r="B23" s="6">
-        <v>1</v>
-      </c>
-      <c r="C23" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="5">
-        <v>23</v>
-      </c>
-      <c r="B24" s="6">
-        <v>2</v>
-      </c>
-      <c r="C24" s="6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="5">
-        <v>24</v>
-      </c>
-      <c r="B25" s="6">
-        <v>3</v>
-      </c>
-      <c r="C25" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="5">
-        <v>25</v>
-      </c>
-      <c r="B26" s="7">
-        <v>4</v>
-      </c>
-      <c r="C26" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="5">
-        <v>26</v>
-      </c>
-      <c r="B27" s="6">
-        <v>5</v>
-      </c>
-      <c r="C27" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="5">
-        <v>27</v>
-      </c>
-      <c r="B28" s="6">
-        <v>6</v>
-      </c>
-      <c r="C28" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="5">
-        <v>28</v>
-      </c>
-      <c r="B29" s="6">
-        <v>7</v>
-      </c>
-      <c r="C29" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="5">
-        <v>29</v>
-      </c>
-      <c r="B30" s="6">
-        <v>2</v>
-      </c>
-      <c r="C30" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="5">
-        <v>30</v>
-      </c>
-      <c r="B31" s="6">
-        <v>3</v>
-      </c>
-      <c r="C31" s="6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="5">
-        <v>31</v>
-      </c>
-      <c r="B32" s="6">
-        <v>4</v>
-      </c>
-      <c r="C32" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="5">
-        <v>32</v>
-      </c>
-      <c r="B33" s="6">
-        <v>5</v>
-      </c>
-      <c r="C33" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="5">
-        <v>33</v>
-      </c>
-      <c r="B34" s="6">
-        <v>6</v>
-      </c>
-      <c r="C34" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="5">
-        <v>34</v>
-      </c>
-      <c r="B35" s="6">
-        <v>7</v>
-      </c>
-      <c r="C35" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="5">
-        <v>35</v>
-      </c>
-      <c r="B36" s="6">
-        <v>8</v>
-      </c>
-      <c r="C36" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="5">
-        <v>36</v>
-      </c>
-      <c r="B37" s="6">
-        <v>3</v>
-      </c>
-      <c r="C37" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="5">
-        <v>37</v>
-      </c>
-      <c r="B38" s="6">
-        <v>4</v>
-      </c>
-      <c r="C38" s="6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="5">
-        <v>38</v>
-      </c>
-      <c r="B39" s="6">
-        <v>5</v>
-      </c>
-      <c r="C39" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="5">
-        <v>39</v>
-      </c>
-      <c r="B40" s="6">
-        <v>6</v>
-      </c>
-      <c r="C40" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="5">
-        <v>40</v>
-      </c>
-      <c r="B41" s="5">
-        <v>7</v>
-      </c>
-      <c r="C41" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="5">
-        <v>41</v>
-      </c>
-      <c r="B42" s="5">
-        <v>8</v>
-      </c>
-      <c r="C42" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="5">
-        <v>42</v>
-      </c>
-      <c r="B43" s="5">
-        <v>9</v>
-      </c>
-      <c r="C43" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="5">
-        <v>43</v>
-      </c>
-      <c r="B44" s="5">
-        <v>4</v>
-      </c>
-      <c r="C44" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="5">
-        <v>44</v>
-      </c>
-      <c r="B45" s="5">
-        <v>5</v>
-      </c>
-      <c r="C45" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="5">
-        <v>45</v>
-      </c>
-      <c r="B46" s="5">
-        <v>6</v>
-      </c>
-      <c r="C46" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="5">
-        <v>46</v>
-      </c>
-      <c r="B47" s="5">
-        <v>7</v>
-      </c>
-      <c r="C47" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="5">
-        <v>47</v>
-      </c>
-      <c r="B48" s="5">
-        <v>8</v>
-      </c>
-      <c r="C48" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="5">
-        <v>48</v>
-      </c>
-      <c r="B49" s="5">
-        <v>9</v>
-      </c>
-      <c r="C49" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="5">
-        <v>49</v>
-      </c>
-      <c r="B50" s="5">
-        <v>5</v>
-      </c>
-      <c r="C50" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="5">
-        <v>50</v>
-      </c>
-      <c r="B51" s="5">
-        <v>6</v>
-      </c>
-      <c r="C51" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="5">
-        <v>51</v>
-      </c>
-      <c r="B52" s="5">
-        <v>7</v>
-      </c>
-      <c r="C52" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="5">
-        <v>52</v>
-      </c>
-      <c r="B53" s="5">
-        <v>8</v>
-      </c>
-      <c r="C53" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="5">
-        <v>53</v>
-      </c>
-      <c r="B54" s="5">
-        <v>9</v>
-      </c>
-      <c r="C54" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="5">
-        <v>54</v>
-      </c>
-      <c r="B55" s="5">
-        <v>6</v>
-      </c>
-      <c r="C55" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="5">
-        <v>55</v>
-      </c>
-      <c r="B56" s="5">
-        <v>7</v>
-      </c>
-      <c r="C56" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="5">
-        <v>56</v>
-      </c>
-      <c r="B57" s="5">
-        <v>8</v>
-      </c>
-      <c r="C57" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="5">
-        <v>57</v>
-      </c>
-      <c r="B58" s="5">
-        <v>9</v>
-      </c>
-      <c r="C58" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="5">
-        <v>58</v>
-      </c>
-      <c r="B59" s="5">
-        <v>7</v>
-      </c>
-      <c r="C59" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="5">
-        <v>59</v>
-      </c>
-      <c r="B60" s="5">
-        <v>8</v>
-      </c>
-      <c r="C60" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="5">
-        <v>60</v>
-      </c>
-      <c r="B61" s="5">
-        <v>9</v>
-      </c>
-      <c r="C61" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="5">
-        <v>61</v>
-      </c>
-      <c r="B62" s="5">
-        <v>8</v>
-      </c>
-      <c r="C62" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="5">
-        <v>62</v>
-      </c>
-      <c r="B63" s="5">
-        <v>9</v>
-      </c>
-      <c r="C63" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="5">
-        <v>63</v>
-      </c>
-      <c r="B64" s="5">
-        <v>9</v>
-      </c>
-      <c r="C64" s="5">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03A5829A-45FE-ED49-88D5-6196BA917271}">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="2" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
 </file>
</xml_diff>